<commit_message>
added resistors as per chris edits
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D0136E-C9A7-A243-AEB5-1D1BCCCF184A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8642413C-3950-9A43-A8AD-0BEE49647803}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
+    <workbookView xWindow="1240" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="162">
   <si>
     <t>ID</t>
   </si>
@@ -517,6 +517,9 @@
   </si>
   <si>
     <t>Looks available. Terrie has talked</t>
+  </si>
+  <si>
+    <t>108-PLP16-C1RD3-SE6-ND</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1162,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1670,7 +1673,7 @@
         <v>62</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>77</v>
+        <v>161</v>
       </c>
       <c r="F19" s="33" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
version ordered V2 - need to annotate schematic
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8642413C-3950-9A43-A8AD-0BEE49647803}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4541025B-7C6A-A341-8EDF-52498AEF659D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="166">
   <si>
     <t>ID</t>
   </si>
@@ -520,6 +520,18 @@
   </si>
   <si>
     <t>108-PLP16-C1RD3-SE6-ND</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>RC0805JR-071KL</t>
+  </si>
+  <si>
+    <t>311-1.0KARTR-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/RC0805JR-071KL/311-1-0KARTR-ND/728218</t>
   </si>
 </sst>
 </file>
@@ -1161,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB09F318-339D-2C4D-BE3F-E973DAF25A4A}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1487,60 +1499,49 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
-      <c r="B12" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="9">
-        <f>10+6+8</f>
-        <v>24</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="16">
-        <v>20390000</v>
-      </c>
+      <c r="B12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="1">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>74</v>
+        <f>10+6+8</f>
+        <v>24</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>72</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="9"/>
       <c r="I13" s="16">
-        <v>4000</v>
-      </c>
-      <c r="J13" s="1">
-        <v>15</v>
+        <v>20390000</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1548,26 +1549,55 @@
         <v>82</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
       </c>
       <c r="D14" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="16">
+        <v>4000</v>
+      </c>
+      <c r="J14" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E15" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="16">
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="16">
         <v>4500</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J15" s="1">
         <v>20</v>
       </c>
     </row>
@@ -1575,11 +1605,6 @@
       <c r="A16" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="D16" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="F16" s="4"/>
       <c r="O16" s="18" t="s">
         <v>143</v>
       </c>
@@ -1590,31 +1615,15 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="I17" s="28">
-        <v>2</v>
-      </c>
+      <c r="B17" s="18"/>
+      <c r="D17" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="4"/>
       <c r="O17" s="29" t="s">
         <v>149</v>
       </c>
@@ -1625,31 +1634,30 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>125</v>
+      <c r="B18" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="1" t="s">
-        <v>137</v>
+      <c r="F18" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="I18" s="28">
+        <v>2</v>
       </c>
       <c r="O18" s="18" t="s">
         <v>150</v>
@@ -1661,30 +1669,31 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="17">
-        <v>60</v>
-      </c>
-      <c r="J19" s="1">
-        <v>8</v>
+      <c r="B19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="O19" s="18" t="s">
         <v>150</v>
@@ -1696,53 +1705,53 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>126</v>
-      </c>
+      <c r="B20" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="32"/>
+      <c r="H20" s="34"/>
       <c r="I20" s="17">
-        <v>0</v>
-      </c>
-      <c r="J20" s="25" t="s">
-        <v>128</v>
+        <v>60</v>
+      </c>
+      <c r="J20" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>104</v>
+      <c r="B21" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>130</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I21" s="19">
-        <v>758</v>
-      </c>
-      <c r="J21" s="1">
-        <v>15</v>
+        <v>127</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>128</v>
       </c>
       <c r="K21" s="18" t="s">
         <v>124</v>
@@ -1755,24 +1764,26 @@
       <c r="A22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>56</v>
+      <c r="B22" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>57</v>
+        <v>105</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="I22" s="16">
-        <v>35000</v>
+        <v>103</v>
+      </c>
+      <c r="I22" s="19">
+        <v>758</v>
+      </c>
+      <c r="J22" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -1780,73 +1791,68 @@
         <v>134</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="I23" s="16">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="I23" s="16">
+      <c r="G24" s="8"/>
+      <c r="I24" s="16">
         <v>7500</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J24" s="1">
         <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C24" s="9">
-        <v>1</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="4" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>63</v>
       </c>
+      <c r="C25" s="9">
+        <v>1</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="4" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="I26" s="17">
-        <v>100</v>
-      </c>
-      <c r="J26" s="1">
-        <v>8</v>
-      </c>
       <c r="K26" s="1" t="s">
         <v>121</v>
       </c>
@@ -1855,31 +1861,57 @@
       <c r="A27" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="17">
+        <v>100</v>
+      </c>
+      <c r="J27" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B28" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C28" s="9">
         <v>1</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D28" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E28" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9" t="s">
+      <c r="G28" s="9"/>
+      <c r="H28" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="I27" s="16">
+      <c r="I28" s="16">
         <v>15000</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="I28" s="27"/>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="I29" s="27"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B30" s="9"/>
@@ -1979,26 +2011,27 @@
     <hyperlink ref="F2" r:id="rId1" xr:uid="{7B5E6841-F24D-4947-8083-A02BA6A18D01}"/>
     <hyperlink ref="F9" r:id="rId2" display="https://www.digikey.com/product-detail/en/vishay-siliconix/2N7002E-T1-E3/2N7002E-T1-E3CT-ND/3946142?utm_adgroup=Semiconductor%20Modules&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_RLSA_Buyers&amp;utm_term=&amp;utm_content=Semiconductor%20Modules&amp;gclid=Cj0KCQjwrIf3BRD1ARIsAMuugNtAYg0B4uzN6uG3FDVYlywiEKFAGbXRLO8hnfXG_d9twvCOg1_5j4waAs4CEALw_wcB" xr:uid="{018F482C-2DD5-9342-BF3B-059DF1382044}"/>
     <hyperlink ref="F10" r:id="rId3" xr:uid="{EBFDAA92-0578-9C4B-8A60-D7469E23F226}"/>
-    <hyperlink ref="F12" r:id="rId4" xr:uid="{8FB55559-59B6-1A4D-915E-15D7A3746398}"/>
-    <hyperlink ref="F22" r:id="rId5" xr:uid="{CE820B91-A3E0-FF4C-86ED-FA1B9A9674A2}"/>
+    <hyperlink ref="F13" r:id="rId4" xr:uid="{8FB55559-59B6-1A4D-915E-15D7A3746398}"/>
+    <hyperlink ref="F23" r:id="rId5" xr:uid="{CE820B91-A3E0-FF4C-86ED-FA1B9A9674A2}"/>
     <hyperlink ref="F41" r:id="rId6" xr:uid="{DF12FEDB-0DDC-2948-8CA6-24D3CDAE683B}"/>
     <hyperlink ref="F3" r:id="rId7" xr:uid="{3123A9C7-DDA3-1247-B2C0-2639E0E65E57}"/>
     <hyperlink ref="F5" r:id="rId8" xr:uid="{F50A23A6-6271-0546-B595-42241E892622}"/>
     <hyperlink ref="F4" r:id="rId9" xr:uid="{FA5DA2F8-8B34-A647-B413-30133DA5F6B0}"/>
     <hyperlink ref="F8" r:id="rId10" xr:uid="{630F37CB-1E8B-C946-90D0-AF7758D45495}"/>
-    <hyperlink ref="F26" r:id="rId11" xr:uid="{951D4A0F-6B66-B347-BB83-79D1699FA1F0}"/>
-    <hyperlink ref="F18" r:id="rId12" xr:uid="{5403C09A-FC9F-4246-86F3-1FB7F3CEC876}"/>
-    <hyperlink ref="F21" r:id="rId13" xr:uid="{BBD95B9F-5EB1-994B-8AFB-B21204AC69EC}"/>
+    <hyperlink ref="F27" r:id="rId11" xr:uid="{951D4A0F-6B66-B347-BB83-79D1699FA1F0}"/>
+    <hyperlink ref="F19" r:id="rId12" xr:uid="{5403C09A-FC9F-4246-86F3-1FB7F3CEC876}"/>
+    <hyperlink ref="F22" r:id="rId13" xr:uid="{BBD95B9F-5EB1-994B-8AFB-B21204AC69EC}"/>
     <hyperlink ref="F6" r:id="rId14" xr:uid="{ABF3B3FB-D57E-DF4C-A3BB-1F1EE7F004E6}"/>
     <hyperlink ref="F11" r:id="rId15" xr:uid="{42296486-DCA2-8147-BAAA-50841A3237D4}"/>
-    <hyperlink ref="F13" r:id="rId16" xr:uid="{3ECE82A6-165C-C746-9108-F3C5C47C845B}"/>
-    <hyperlink ref="F14" r:id="rId17" xr:uid="{E7AAA494-615C-634D-B386-4AE6FBEEE153}"/>
-    <hyperlink ref="F23" r:id="rId18" xr:uid="{D037F001-3F77-824D-8684-B324825BB7B8}"/>
-    <hyperlink ref="F27" r:id="rId19" xr:uid="{12B930BB-688C-8646-9406-D989687BBC42}"/>
-    <hyperlink ref="G20" r:id="rId20" xr:uid="{0B23E427-31CE-5244-A415-19CBF752FC9D}"/>
-    <hyperlink ref="F19" r:id="rId21" xr:uid="{0376E0AC-73E1-B441-9DE3-A2BA1839C66A}"/>
+    <hyperlink ref="F14" r:id="rId16" xr:uid="{3ECE82A6-165C-C746-9108-F3C5C47C845B}"/>
+    <hyperlink ref="F15" r:id="rId17" xr:uid="{E7AAA494-615C-634D-B386-4AE6FBEEE153}"/>
+    <hyperlink ref="F24" r:id="rId18" xr:uid="{D037F001-3F77-824D-8684-B324825BB7B8}"/>
+    <hyperlink ref="F28" r:id="rId19" xr:uid="{12B930BB-688C-8646-9406-D989687BBC42}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{0B23E427-31CE-5244-A415-19CBF752FC9D}"/>
+    <hyperlink ref="F20" r:id="rId21" xr:uid="{0376E0AC-73E1-B441-9DE3-A2BA1839C66A}"/>
     <hyperlink ref="F32" r:id="rId22" xr:uid="{B3713357-F350-1B47-88EA-259846C28AEC}"/>
-    <hyperlink ref="F17" r:id="rId23" xr:uid="{B166558D-0EEC-DB45-892C-783F7EE842FA}"/>
+    <hyperlink ref="F18" r:id="rId23" xr:uid="{B166558D-0EEC-DB45-892C-783F7EE842FA}"/>
+    <hyperlink ref="F12" r:id="rId24" xr:uid="{EF6D6457-CC43-8041-AF01-7801FE618C7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
assembly changes (footprint, etc)
</commit_message>
<xml_diff>
--- a/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2.xlsx
+++ b/designs/Pufferfish-Interface-2/reference/Interface Bill of Materials v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenadachi/Documents/GitHub/pufferfish-electronics/designs/Pufferfish-Interface-2/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4541025B-7C6A-A341-8EDF-52498AEF659D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5D468B-4C85-9A4D-8EBC-B8F679FE1C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="25040" windowHeight="14040" xr2:uid="{AB4FADCF-5D3E-0F4F-A6DE-656B770204FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="165">
   <si>
     <t>ID</t>
   </si>
@@ -522,23 +522,20 @@
     <t>108-PLP16-C1RD3-SE6-ND</t>
   </si>
   <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>RC0805JR-071KL</t>
-  </si>
-  <si>
-    <t>311-1.0KARTR-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/yageo/RC0805JR-071KL/311-1-0KARTR-ND/728218</t>
+    <t>https://www.digikey.com/product-detail/en/yageo/RC0805FR-071RL/311-1-00CRCT-ND/730390</t>
+  </si>
+  <si>
+    <t>RC0805FR-071RL</t>
+  </si>
+  <si>
+    <t>311-1.00CRCT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -740,6 +737,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -792,7 +801,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -856,6 +865,13 @@
     <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1173,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB09F318-339D-2C4D-BE3F-E973DAF25A4A}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1367,7 +1383,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>96</v>
       </c>
@@ -1383,7 +1399,7 @@
       <c r="E7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="53" t="s">
         <v>112</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1396,7 +1412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -1412,7 +1428,7 @@
       <c r="E8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="56" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="16">
@@ -1497,24 +1513,24 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:18" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="55">
         <v>19</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="57">
+        <v>1</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="11"/>
+      <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
@@ -1731,10 +1747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="26" t="s">
-        <v>132</v>
-      </c>
+    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="25" t="s">
         <v>129</v>
       </c>
@@ -1744,7 +1757,7 @@
       <c r="F21" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="53" t="s">
         <v>126</v>
       </c>
       <c r="I21" s="17">
@@ -1761,8 +1774,8 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>133</v>
+      <c r="A22" s="26" t="s">
+        <v>132</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>104</v>
@@ -1788,7 +1801,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>56</v>
@@ -1811,6 +1824,9 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="B24" s="1" t="s">
         <v>83</v>
       </c>
@@ -1835,9 +1851,6 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
-        <v>63</v>
-      </c>
       <c r="C25" s="9">
         <v>1</v>
       </c>
@@ -1850,16 +1863,16 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>68</v>
+      <c r="A26" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>67</v>
+      <c r="A27" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>106</v>
@@ -1887,6 +1900,9 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="B28" s="18" t="s">
         <v>107</v>
       </c>
@@ -2031,7 +2047,8 @@
     <hyperlink ref="F20" r:id="rId21" xr:uid="{0376E0AC-73E1-B441-9DE3-A2BA1839C66A}"/>
     <hyperlink ref="F32" r:id="rId22" xr:uid="{B3713357-F350-1B47-88EA-259846C28AEC}"/>
     <hyperlink ref="F18" r:id="rId23" xr:uid="{B166558D-0EEC-DB45-892C-783F7EE842FA}"/>
-    <hyperlink ref="F12" r:id="rId24" xr:uid="{EF6D6457-CC43-8041-AF01-7801FE618C7B}"/>
+    <hyperlink ref="F12" r:id="rId24" xr:uid="{0B85D746-5546-E541-84B9-9793C43877D8}"/>
+    <hyperlink ref="F7" r:id="rId25" xr:uid="{C421FEF6-4573-DF4F-9704-042BBC804F34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>